<commit_message>
WBCAMS-1502: [AMS] Update SSOT with September Monthly Labour Force Survey data
</commit_message>
<xml_diff>
--- a/migration/data/WorkBC LMS September_2025.xlsx
+++ b/migration/data/WorkBC LMS September_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebaydar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\7. WORKBC and PROJECTS\LMI Data Updates\Monthly Labour Force Survey\Drupal\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5058F9A8-E16A-4EE2-B90C-D33FD8224D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645D7C4E-B92B-41D1-9F4B-9913C9DA9873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me first" sheetId="4" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>BC Employment Trends</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>September  2024</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -1738,14 +1741,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBC98A6-26E3-4693-9BA5-07FBC64A5104}">
-  <dimension ref="A1"/>
+  <dimension ref="J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="7" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1755,33 +1764,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>45925</v>
       </c>
@@ -1793,7 +1802,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="E4" s="49"/>
@@ -1802,7 +1811,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="E5" s="49"/>
@@ -1812,7 +1821,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
         <v>42</v>
       </c>
@@ -1826,7 +1835,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>49</v>
       </c>
@@ -1844,7 +1853,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>43</v>
       </c>
@@ -1863,7 +1872,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>44</v>
       </c>
@@ -1881,7 +1890,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>45</v>
       </c>
@@ -1897,7 +1906,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>48</v>
       </c>
@@ -1907,7 +1916,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>46</v>
       </c>
@@ -1922,7 +1931,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>47</v>
       </c>
@@ -1940,7 +1949,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="17"/>
       <c r="E14" s="21"/>
@@ -1951,7 +1960,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="56" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1973,7 @@
       <c r="K15" s="16"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
         <v>55</v>
@@ -1979,7 +1988,7 @@
       <c r="K16" s="16"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
@@ -1997,7 +2006,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>9</v>
       </c>
@@ -2019,7 +2028,7 @@
       <c r="K18" s="16"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -2041,7 +2050,7 @@
       <c r="K19" s="16"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2072,7 @@
       <c r="K20" s="16"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>40</v>
       </c>
@@ -2080,7 +2089,7 @@
       <c r="K21" s="16"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>12</v>
       </c>
@@ -2100,7 +2109,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>13</v>
       </c>
@@ -2120,12 +2129,12 @@
       <c r="J23" s="20"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="J24" s="20"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="57" t="s">
         <v>2</v>
       </c>
@@ -2135,7 +2144,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="39" t="s">
         <v>7</v>
       </c>
@@ -2151,7 +2160,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>32</v>
       </c>
@@ -2171,7 +2180,7 @@
       <c r="O27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2198,7 @@
       <c r="O28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>19</v>
       </c>
@@ -2207,7 +2216,7 @@
       <c r="O29" s="4"/>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>15</v>
       </c>
@@ -2225,7 +2234,7 @@
       <c r="O30" s="4"/>
       <c r="Q30" s="4"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>14</v>
       </c>
@@ -2242,7 +2251,7 @@
       <c r="L31" s="16"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>17</v>
       </c>
@@ -2258,7 +2267,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
         <v>18</v>
       </c>
@@ -2273,7 +2282,7 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34" s="18"/>
       <c r="F34" s="4"/>
       <c r="G34" s="20"/>
@@ -2283,7 +2292,7 @@
       <c r="K34" s="16"/>
       <c r="L34" s="16"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
         <v>50</v>
       </c>
@@ -2296,7 +2305,7 @@
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
         <v>54</v>
       </c>
@@ -2312,7 +2321,7 @@
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="37">
         <v>195600</v>
       </c>
@@ -2326,13 +2335,13 @@
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
       <c r="H38" s="20"/>
       <c r="J38" s="20"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="58" t="s">
         <v>37</v>
       </c>
@@ -2345,7 +2354,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="16"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="32" t="s">
         <v>53</v>
@@ -2362,7 +2371,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="16"/>
     </row>
-    <row r="41" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>7</v>
       </c>
@@ -2387,7 +2396,7 @@
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>20</v>
       </c>
@@ -2413,7 +2422,7 @@
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>16</v>
       </c>
@@ -2439,7 +2448,7 @@
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>19</v>
       </c>
@@ -2465,7 +2474,7 @@
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30" t="s">
         <v>15</v>
       </c>
@@ -2491,7 +2500,7 @@
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30" t="s">
         <v>14</v>
       </c>
@@ -2516,7 +2525,7 @@
       <c r="O46" s="16"/>
       <c r="P46" s="16"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>17</v>
       </c>
@@ -2541,7 +2550,7 @@
       <c r="P47" s="16"/>
       <c r="Q47" s="16"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30" t="s">
         <v>18</v>
       </c>
@@ -2566,7 +2575,7 @@
       <c r="P48" s="16"/>
       <c r="Q48" s="16"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B49"/>
       <c r="H49" s="4"/>
       <c r="J49" s="4"/>
@@ -2576,7 +2585,7 @@
       <c r="O49" s="16"/>
       <c r="P49" s="16"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="C50" s="6"/>
       <c r="D50" s="16"/>
@@ -2590,7 +2599,7 @@
       <c r="S50" s="16"/>
       <c r="T50" s="16"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="C51" s="5"/>
       <c r="D51" s="16"/>
@@ -2601,7 +2610,7 @@
       <c r="J51" s="4"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="C52" s="5"/>
       <c r="E52" s="22"/>
@@ -2611,7 +2620,7 @@
       <c r="J52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="C53" s="5"/>
       <c r="E53" s="22"/>
@@ -2623,7 +2632,7 @@
       <c r="L53" s="4"/>
       <c r="N53" s="11"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="C54" s="5"/>
       <c r="E54" s="23"/>
@@ -2633,7 +2642,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2642,14 +2651,14 @@
       <c r="H55" s="4"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="4"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="55" t="s">
         <v>21</v>
       </c>
@@ -2662,7 +2671,7 @@
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="30"/>
       <c r="B58" s="38" t="s">
         <v>38</v>
@@ -2679,7 +2688,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="16"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="42" t="s">
         <v>22</v>
       </c>
@@ -2699,7 +2708,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="16"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="42" t="s">
         <v>3</v>
       </c>
@@ -2720,7 +2729,7 @@
       <c r="L60" s="48"/>
       <c r="M60" s="16"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
         <v>6</v>
       </c>
@@ -2740,7 +2749,7 @@
       <c r="L61" s="48"/>
       <c r="M61" s="16"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="42" t="s">
         <v>23</v>
       </c>
@@ -2760,7 +2769,7 @@
       <c r="L62" s="48"/>
       <c r="M62" s="16"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="42" t="s">
         <v>26</v>
       </c>
@@ -2781,7 +2790,7 @@
       <c r="L63" s="48"/>
       <c r="M63" s="16"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="42" t="s">
         <v>29</v>
       </c>
@@ -2802,7 +2811,7 @@
       <c r="L64" s="48"/>
       <c r="M64" s="16"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="42" t="s">
         <v>5</v>
       </c>
@@ -2823,7 +2832,7 @@
       <c r="L65" s="48"/>
       <c r="M65" s="16"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="30" t="s">
         <v>8</v>
       </c>
@@ -2844,7 +2853,7 @@
       <c r="L66" s="48"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="42" t="s">
         <v>28</v>
       </c>
@@ -2865,7 +2874,7 @@
       <c r="L67" s="48"/>
       <c r="M67" s="16"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="42" t="s">
         <v>30</v>
       </c>
@@ -2886,7 +2895,7 @@
       <c r="L68" s="48"/>
       <c r="M68" s="16"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="42" t="s">
         <v>27</v>
       </c>
@@ -2907,7 +2916,7 @@
       <c r="L69" s="48"/>
       <c r="M69" s="16"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="42" t="s">
         <v>24</v>
       </c>
@@ -2928,7 +2937,7 @@
       <c r="L70" s="48"/>
       <c r="M70" s="16"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="42" t="s">
         <v>4</v>
       </c>
@@ -2949,7 +2958,7 @@
       <c r="L71" s="48"/>
       <c r="M71" s="16"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="42" t="s">
         <v>25</v>
       </c>
@@ -2970,7 +2979,7 @@
       <c r="L72" s="48"/>
       <c r="M72" s="16"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="42" t="s">
         <v>51</v>
       </c>
@@ -2991,7 +3000,7 @@
       <c r="L73" s="48"/>
       <c r="M73" s="16"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="42" t="s">
         <v>52</v>
       </c>
@@ -3012,7 +3021,7 @@
       <c r="L74" s="48"/>
       <c r="M74" s="16"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B75" s="12"/>
       <c r="E75" s="22"/>
       <c r="F75" s="20"/>
@@ -3024,14 +3033,14 @@
       <c r="L75" s="48"/>
       <c r="M75" s="16"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F76" s="20"/>
       <c r="G76" s="20"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>34</v>
       </c>
@@ -3040,7 +3049,7 @@
       <c r="H77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>35</v>
       </c>
@@ -3048,7 +3057,7 @@
       <c r="J78" s="15"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>36</v>
       </c>
@@ -3057,7 +3066,7 @@
       <c r="P79" s="16"/>
       <c r="Q79" s="16"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>33</v>
       </c>
@@ -3069,7 +3078,7 @@
       <c r="Q80" s="16"/>
       <c r="R80" s="16"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="J81" s="16"/>
       <c r="K81" s="16"/>
@@ -3079,7 +3088,7 @@
       <c r="Q81" s="16"/>
       <c r="R81" s="16"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="J82" s="16"/>
       <c r="K82" s="16"/>
@@ -3089,82 +3098,82 @@
       <c r="Q82" s="16"/>
       <c r="R82" s="16"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="10"/>
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -3191,23 +3200,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006256975931115C42B154129ACF64F69B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6a5bc4137ad5000bb33d4b302e37fb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xmlns:ns4="6dacf12f-1e0d-46b0-91bd-702888a65233" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b711ee3334e61d74dbc2f1f205886f71" ns3:_="" ns4:_="">
     <xsd:import namespace="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
@@ -3434,32 +3426,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077B7BF1-CF95-434E-B6DF-F71248C924F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6dacf12f-1e0d-46b0-91bd-702888a65233"/>
-    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AD9A7D-2FC8-4FCE-A291-642EFDF647E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDCFECB7-D025-4DEB-B1C9-7FD71B9730FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3476,4 +3460,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AD9A7D-2FC8-4FCE-A291-642EFDF647E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077B7BF1-CF95-434E-B6DF-F71248C924F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6dacf12f-1e0d-46b0-91bd-702888a65233"/>
+    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>